<commit_message>
work number 4 done
</commit_message>
<xml_diff>
--- a/Л4/Формула Бернулли.xlsx
+++ b/Л4/Формула Бернулли.xlsx
@@ -338,11 +338,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="132479616"/>
-        <c:axId val="132478080"/>
+        <c:axId val="142270848"/>
+        <c:axId val="142272384"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132479616"/>
+        <c:axId val="142270848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -352,12 +352,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132478080"/>
+        <c:crossAx val="142272384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132478080"/>
+        <c:axId val="142272384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132479616"/>
+        <c:crossAx val="142270848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -642,11 +642,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="36591872"/>
-        <c:axId val="36590336"/>
+        <c:axId val="142985088"/>
+        <c:axId val="142986624"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="36591872"/>
+        <c:axId val="142985088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -656,12 +656,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36590336"/>
+        <c:crossAx val="142986624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="36590336"/>
+        <c:axId val="142986624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -672,7 +672,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="36591872"/>
+        <c:crossAx val="142985088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -953,11 +953,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="132046208"/>
-        <c:axId val="132044672"/>
+        <c:axId val="169545088"/>
+        <c:axId val="169555072"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="132046208"/>
+        <c:axId val="169545088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -967,12 +967,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132044672"/>
+        <c:crossAx val="169555072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="132044672"/>
+        <c:axId val="169555072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -983,7 +983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132046208"/>
+        <c:crossAx val="169545088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1009,16 +1009,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>366712</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>271462</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>61912</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>576262</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:rowOff>61912</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1039,16 +1039,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>357187</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>233362</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>100012</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>52387</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>538162</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>176212</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1069,16 +1069,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>214312</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>80962</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>519112</xdr:colOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>385762</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>52387</xdr:rowOff>
+      <xdr:rowOff>109537</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1387,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="A1:A32 D1:D32"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,15 +1434,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" ref="B3:B32" si="0">_xlfn.BINOM.DIST(A3,30,0.7,0)</f>
+        <f t="shared" ref="B3:B52" si="0">_xlfn.BINOM.DIST(A3,30,0.7,0)</f>
         <v>1.4412379246625623E-14</v>
       </c>
       <c r="C3" s="2">
-        <f t="shared" ref="C3:C32" si="1">_xlfn.BINOM.DIST(A3,30,0.5,0)</f>
+        <f t="shared" ref="C3:C52" si="1">_xlfn.BINOM.DIST(A3,30,0.5,0)</f>
         <v>2.7939677238464359E-8</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D32" si="2">_xlfn.BINOM.DIST(A3,30,0.2,0)</f>
+        <f t="shared" ref="D3:D52" si="2">_xlfn.BINOM.DIST(A3,30,0.2,0)</f>
         <v>9.2845502946403528E-3</v>
       </c>
     </row>
@@ -1937,6 +1937,346 @@
       <c r="D32" s="2">
         <f t="shared" si="2"/>
         <v>1.0737418240000016E-21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C33" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D33" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C34" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D34" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C35" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D35" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C36" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D36" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C37" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D37" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C38" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D38" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C39" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D39" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C40" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D40" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C41" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D41" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>40</v>
+      </c>
+      <c r="B42" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C42" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D42" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C43" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D43" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C44" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D44" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C45" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D45" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C46" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D46" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C47" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D47" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C48" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D48" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C49" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D49" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C50" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D50" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C51" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D51" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="C52" s="2" t="e">
+        <f t="shared" si="1"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="D52" s="2" t="e">
+        <f t="shared" si="2"/>
+        <v>#NUM!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>